<commit_message>
added a description of the stylized case study on biowaste management
</commit_message>
<xml_diff>
--- a/CaseStudy2_Biowaste/ExcelTool_GeneratorInput_Template.xlsx
+++ b/CaseStudy2_Biowaste/ExcelTool_GeneratorInput_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\CaseStudy2_Biowaste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BED4F8-504A-49FA-8EE1-78B26CC08774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED116F4-AD9F-47C4-91EC-BA40C61EDBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -1006,7 +1006,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="475">
   <si>
     <t>input</t>
   </si>
@@ -2838,6 +2838,9 @@
   </si>
   <si>
     <t>-P3</t>
+  </si>
+  <si>
+    <t>P1</t>
   </si>
 </sst>
 </file>
@@ -3454,15 +3457,6 @@
     <xf numFmtId="2" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3494,6 +3488,15 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3794,9 +3797,9 @@
     <col min="1" max="1" width="27.90625" style="31" customWidth="1"/>
     <col min="2" max="2" width="117.6328125" style="31" customWidth="1"/>
     <col min="3" max="3" width="10.90625" style="31"/>
-    <col min="4" max="6" width="10.90625" style="93"/>
+    <col min="4" max="6" width="10.90625" style="90"/>
     <col min="7" max="11" width="10.90625" style="43"/>
-    <col min="12" max="19" width="10.90625" style="93"/>
+    <col min="12" max="19" width="10.90625" style="90"/>
     <col min="20" max="16384" width="10.90625" style="31"/>
   </cols>
   <sheetData>
@@ -3811,10 +3814,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="101" t="s">
         <v>442</v>
       </c>
-      <c r="B4" s="87"/>
+      <c r="B4" s="101"/>
     </row>
     <row r="6" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
@@ -4052,10 +4055,10 @@
       <c r="B2" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="91">
+      <c r="D2" s="88">
         <v>8400</v>
       </c>
       <c r="E2" s="25" t="s">
@@ -4075,10 +4078,10 @@
       <c r="B3" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="87" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="91">
+      <c r="D3" s="88">
         <v>2.3400000000000001E-2</v>
       </c>
       <c r="E3" s="25" t="s">
@@ -4098,10 +4101,10 @@
       <c r="B4" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="91">
+      <c r="D4" s="88">
         <v>3.8500000000000001E-5</v>
       </c>
       <c r="E4" s="25" t="s">
@@ -4121,10 +4124,10 @@
       <c r="B5" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="91">
+      <c r="D5" s="88">
         <v>4.75E-4</v>
       </c>
       <c r="E5" s="25" t="s">
@@ -4144,10 +4147,10 @@
       <c r="B6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="91">
+      <c r="D6" s="88">
         <v>7.18E-4</v>
       </c>
       <c r="E6" s="25" t="s">
@@ -4167,10 +4170,10 @@
       <c r="B7" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="87" t="s">
         <v>154</v>
       </c>
-      <c r="D7" s="91">
+      <c r="D7" s="88">
         <v>4220</v>
       </c>
       <c r="E7" s="25" t="s">
@@ -4190,10 +4193,10 @@
       <c r="B8" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="C8" s="87" t="s">
         <v>155</v>
       </c>
-      <c r="D8" s="91">
+      <c r="D8" s="88">
         <v>40.6</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -4213,10 +4216,10 @@
       <c r="B9" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="D9" s="91">
+      <c r="D9" s="88">
         <v>55.5</v>
       </c>
       <c r="E9" s="25" t="s">
@@ -4236,10 +4239,10 @@
       <c r="B10" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="87" t="s">
         <v>157</v>
       </c>
-      <c r="D10" s="91">
+      <c r="D10" s="88">
         <v>177</v>
       </c>
       <c r="E10" s="25" t="s">
@@ -4259,10 +4262,10 @@
       <c r="B11" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="87" t="s">
         <v>158</v>
       </c>
-      <c r="D11" s="91">
+      <c r="D11" s="88">
         <v>0.73399999999999999</v>
       </c>
       <c r="E11" s="25" t="s">
@@ -4282,10 +4285,10 @@
       <c r="B12" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="91">
+      <c r="D12" s="88">
         <v>28.3</v>
       </c>
       <c r="E12" s="25" t="s">
@@ -4305,10 +4308,10 @@
       <c r="B13" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="D13" s="91">
+      <c r="D13" s="88">
         <v>11800</v>
       </c>
       <c r="E13" s="25" t="s">
@@ -4328,10 +4331,10 @@
       <c r="B14" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="87" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="91">
+      <c r="D14" s="88">
         <v>1400000</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -4351,10 +4354,10 @@
       <c r="B15" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="89" t="s">
         <v>162</v>
       </c>
-      <c r="D15" s="91">
+      <c r="D15" s="88">
         <v>11500</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -4374,10 +4377,10 @@
       <c r="B16" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="90" t="s">
+      <c r="C16" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="D16" s="91">
+      <c r="D16" s="88">
         <v>6.3600000000000004E-2</v>
       </c>
       <c r="E16" s="25" t="s">
@@ -4397,10 +4400,10 @@
       <c r="B17" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="90" t="s">
+      <c r="C17" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="D17" s="91">
+      <c r="D17" s="88">
         <v>65300</v>
       </c>
       <c r="E17" s="25" t="s">
@@ -5835,10 +5838,10 @@
       </c>
     </row>
     <row r="4" spans="1:11" s="35" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="101" t="s">
         <v>442</v>
       </c>
-      <c r="B4" s="87"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -5976,10 +5979,10 @@
       <c r="K14" s="43"/>
     </row>
     <row r="15" spans="1:11" s="35" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="102" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="89"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -7143,7 +7146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -7250,7 +7253,7 @@
       <c r="I3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="101" t="s">
+      <c r="J3" s="98" t="s">
         <v>469</v>
       </c>
     </row>
@@ -7282,7 +7285,7 @@
       <c r="I4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="101" t="s">
+      <c r="J4" s="98" t="s">
         <v>470</v>
       </c>
     </row>
@@ -7644,7 +7647,7 @@
       <c r="I16" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="102" t="s">
+      <c r="J16" s="99" t="s">
         <v>472</v>
       </c>
     </row>
@@ -7676,7 +7679,7 @@
       <c r="I17" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="102" t="s">
+      <c r="J17" s="99" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7800,7 +7803,7 @@
       <c r="I21" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="103" t="s">
+      <c r="J21" s="100" t="s">
         <v>472</v>
       </c>
     </row>
@@ -7832,7 +7835,7 @@
       <c r="I22" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="100" t="s">
         <v>473</v>
       </c>
     </row>
@@ -10548,84 +10551,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40A9123-B5A2-440C-9957-36B1335A3358}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="95" customWidth="1"/>
-    <col min="2" max="2" width="34.1796875" style="95" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" style="95" customWidth="1"/>
-    <col min="4" max="4" width="15" style="95" customWidth="1"/>
-    <col min="5" max="16384" width="10.90625" style="95"/>
+    <col min="1" max="1" width="13.81640625" style="92" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" style="92" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" style="92" customWidth="1"/>
+    <col min="4" max="4" width="15" style="92" customWidth="1"/>
+    <col min="5" max="16384" width="10.90625" style="92"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="93" t="s">
         <v>440</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="93" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="93" t="s">
         <v>441</v>
       </c>
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="91" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="94" t="s">
+        <v>474</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="97">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="E2" s="94" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="94" t="s">
         <v>462</v>
       </c>
-      <c r="B2" s="97" t="s">
-        <v>463</v>
-      </c>
-      <c r="C2" s="100">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="99" t="s">
+      <c r="B3" s="95" t="s">
+        <v>464</v>
+      </c>
+      <c r="C3" s="97">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="96" t="s">
         <v>467</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E3" s="94" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+    <row r="4" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="94" t="s">
         <v>465</v>
       </c>
-      <c r="B3" s="98" t="s">
-        <v>464</v>
-      </c>
-      <c r="C3" s="100">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="99" t="s">
-        <v>467</v>
-      </c>
-      <c r="E3" s="97" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
-        <v>471</v>
-      </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="95" t="s">
         <v>466</v>
       </c>
-      <c r="C4" s="97">
+      <c r="C4" s="94">
         <v>0.1</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="94" t="s">
         <v>468</v>
       </c>
     </row>
@@ -10727,13 +10730,13 @@
       <c r="A1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="103" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -10897,7 +10900,7 @@
         <v>69</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10905,7 +10908,7 @@
         <v>70</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10913,7 +10916,7 @@
         <v>71</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -10921,7 +10924,7 @@
         <v>72</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -10929,7 +10932,7 @@
         <v>73</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -10937,7 +10940,7 @@
         <v>74</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -10945,7 +10948,7 @@
         <v>75</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>